<commit_message>
CC2650 Technical Reference Manual hinzugefügt, Zeitblätter
</commit_message>
<xml_diff>
--- a/Zeitblaetter/Tobias Breuß.xlsx
+++ b/Zeitblaetter/Tobias Breuß.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Datum</t>
   </si>
@@ -806,7 +806,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -870,6 +870,12 @@
         <f t="shared" si="0"/>
         <v>42680</v>
       </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1027,7 +1033,7 @@
       </c>
       <c r="B36" s="2">
         <f>SUM(B5:B34)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>